<commit_message>
modified arbeitsmatrix, changed color of intrface elmements to be consistent
</commit_message>
<xml_diff>
--- a/Artefakte/WS2122_ChouliarasBurgdorfWolf_Arbeitsmatrix_V01.xlsx
+++ b/Artefakte/WS2122_ChouliarasBurgdorfWolf_Arbeitsmatrix_V01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Entwicklungsprojekt\EPW2122ChouliarasBurgdorfWolf\Artefakte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Semester_5\EP\EPW2122ChouliarasBurgdorfWolf\Artefakte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5AD308-9E06-4602-B87D-39EE3CA06267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3917829B-8222-421D-A04B-8DFD5066139D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1650" yWindow="0" windowWidth="25020" windowHeight="16785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
   <si>
     <t>ToDo</t>
   </si>
@@ -166,15 +166,9 @@
     <t>Rapid Prototype</t>
   </si>
   <si>
-    <t>Artefakte</t>
-  </si>
-  <si>
     <t>Anforderungen</t>
   </si>
   <si>
-    <t>Anwendungslogik</t>
-  </si>
-  <si>
     <t>Domänenmodell</t>
   </si>
   <si>
@@ -187,9 +181,6 @@
     <t>Zielhierarchie</t>
   </si>
   <si>
-    <t>PoCs Text und Grafik</t>
-  </si>
-  <si>
     <t>Programmefestlegung</t>
   </si>
   <si>
@@ -208,28 +199,70 @@
     <t>React Implementierung</t>
   </si>
   <si>
-    <t>Umgesetzte Features</t>
-  </si>
-  <si>
-    <t>Grundriss 3D Modell</t>
-  </si>
-  <si>
-    <t>1/3</t>
-  </si>
-  <si>
-    <t>Audits vorbereiten</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>1/4</t>
-  </si>
-  <si>
-    <t>3/4</t>
-  </si>
-  <si>
     <t>Linie/Weg bei Texteingabe</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
+    <t>10%</t>
+  </si>
+  <si>
+    <t>90%</t>
+  </si>
+  <si>
+    <t>3D Modelle</t>
+  </si>
+  <si>
+    <t>33%</t>
+  </si>
+  <si>
+    <t>Auditpräsentation vorbereiten</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>AnwendungslogikDiagramm</t>
+  </si>
+  <si>
+    <t>aSternVariant_Beispiele</t>
+  </si>
+  <si>
+    <t>Expose</t>
+  </si>
+  <si>
+    <t>PoC</t>
+  </si>
+  <si>
+    <t>PocFlow</t>
+  </si>
+  <si>
+    <t>ProgrammGraph</t>
+  </si>
+  <si>
+    <t>Artefaktanfertigung</t>
+  </si>
+  <si>
+    <t>80%</t>
+  </si>
+  <si>
+    <t>Projktideen</t>
+  </si>
+  <si>
+    <t>Pseudocode A Star Variant</t>
+  </si>
+  <si>
+    <t>Pseudocode</t>
+  </si>
+  <si>
+    <t>Risikoanalyse</t>
+  </si>
+  <si>
+    <t>Umgesetzte Features/Intgration</t>
   </si>
 </sst>
 </file>
@@ -315,7 +348,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -381,8 +414,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -757,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D28"/>
+  <dimension ref="A2:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -786,282 +829,356 @@
       <c r="A3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25" t="s">
-        <v>64</v>
+        <v>54</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25" t="s">
-        <v>65</v>
-      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="25"/>
+        <v>56</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="26"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="B10" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
+        <v>78</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
+        <v>72</v>
+      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="25" t="s">
+      <c r="B19" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>62</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>62</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>62</v>
+        <v>49</v>
+      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>62</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="26"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="25" t="s">
-        <v>62</v>
+        <v>51</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="26"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="27">
+        <v>1</v>
+      </c>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="27">
+        <v>1</v>
+      </c>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1074,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866D198E-5AB9-4659-98FE-90D6D40AD3BA}">
   <dimension ref="A2:M24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1432,7 @@
     </row>
     <row r="14" spans="1:13" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Funktionierend mit neuen Aufzügen
</commit_message>
<xml_diff>
--- a/Artefakte/WS2122_ChouliarasBurgdorfWolf_Arbeitsmatrix_V01.xlsx
+++ b/Artefakte/WS2122_ChouliarasBurgdorfWolf_Arbeitsmatrix_V01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Semester_5\EP\EPW2122ChouliarasBurgdorfWolf\Artefakte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Entwicklungsprojekt\EPW2122ChouliarasBurgdorfWolf\Artefakte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3917829B-8222-421D-A04B-8DFD5066139D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24392655-6AC1-4F34-BDD6-28193617E249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="0" windowWidth="25020" windowHeight="16785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -802,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1191,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{866D198E-5AB9-4659-98FE-90D6D40AD3BA}">
   <dimension ref="A2:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>